<commit_message>
Fixed 3D model issues
</commit_message>
<xml_diff>
--- a/Hardware/Part-Footprint Table.xlsx
+++ b/Hardware/Part-Footprint Table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh Johnson\Dropbox\ENGN4200\Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh Johnson\Dropbox\ENGN4200\vna\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1056912A-C544-4426-80C8-099FD28405FC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5DBC88-A131-45EE-90B4-28EE551E4378}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="24750" xr2:uid="{4662F339-0714-44B5-AC0C-A9345AFF81B4}"/>
   </bookViews>
@@ -90,9 +90,6 @@
     <t>Switch SP4T</t>
   </si>
   <si>
-    <t>SKY13380-350LF</t>
-  </si>
-  <si>
     <t>QFN-16-1EP-3x3mm_Pitch0.5mm</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>CD542</t>
+  </si>
+  <si>
+    <t>PE42440</t>
   </si>
 </sst>
 </file>
@@ -466,7 +466,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,32 +546,32 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
         <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
         <v>24</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added FV1206 and DIP switch models and footprints, along with micro USB footprint
</commit_message>
<xml_diff>
--- a/Hardware/Part-Footprint Table.xlsx
+++ b/Hardware/Part-Footprint Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh Johnson\Dropbox\ENGN4200\vna\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5DBC88-A131-45EE-90B4-28EE551E4378}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742D6BFC-DB3E-46EA-B661-FF850E09EBE3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="24750" xr2:uid="{4662F339-0714-44B5-AC0C-A9345AFF81B4}"/>
   </bookViews>
@@ -90,9 +90,6 @@
     <t>Switch SP4T</t>
   </si>
   <si>
-    <t>QFN-16-1EP-3x3mm_Pitch0.5mm</t>
-  </si>
-  <si>
     <t>Gain/Phase Detector</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>PE42440</t>
+  </si>
+  <si>
+    <t>QFN-16-1EP_3x3mm_P0.5mm_EP2.7x2.7mm_ThermalVias</t>
   </si>
 </sst>
 </file>
@@ -466,7 +466,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,32 +546,32 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
         <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated functionals with new power detector
</commit_message>
<xml_diff>
--- a/Hardware/Part-Footprint Table.xlsx
+++ b/Hardware/Part-Footprint Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh Johnson\Dropbox\ENGN4200\vna\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742D6BFC-DB3E-46EA-B661-FF850E09EBE3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34099B0-5825-427E-A046-D47137332AA2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="24750" xr2:uid="{4662F339-0714-44B5-AC0C-A9345AFF81B4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Part Number</t>
   </si>
@@ -63,12 +63,6 @@
     <t>Power Detector</t>
   </si>
   <si>
-    <t>MAX9933</t>
-  </si>
-  <si>
-    <t>8 uMax</t>
-  </si>
-  <si>
     <t>QFN-24-1EP-4x4mm_Pitch0.5mm</t>
   </si>
   <si>
@@ -112,6 +106,9 @@
   </si>
   <si>
     <t>QFN-16-1EP_3x3mm_P0.5mm_EP2.7x2.7mm_ThermalVias</t>
+  </si>
+  <si>
+    <t>AD8319</t>
   </si>
 </sst>
 </file>
@@ -466,7 +463,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,65 +510,62 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
         <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
         <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
         <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>